<commit_message>
parent can be non-distinct
</commit_message>
<xml_diff>
--- a/write-ups/cikm/clustering.xlsx
+++ b/write-ups/cikm/clustering.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="28560" windowHeight="15400" tabRatio="500" firstSheet="10" activeTab="14"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="28560" windowHeight="15400" tabRatio="500" firstSheet="10" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="BUGGY_Jaccard+NoCos" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="HandOpt_JaccardVs" sheetId="13" r:id="rId13"/>
     <sheet name="SimConf_all" sheetId="14" r:id="rId14"/>
     <sheet name="RuntimeHandOptJaccard" sheetId="15" r:id="rId15"/>
+    <sheet name="ClustClosed=ParentClosed" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="289">
   <si>
     <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_oct-nov-dec/, Jaccard+NoCos_conf0.1_Buff1000,  ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=0.66 ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.1]</t>
   </si>
@@ -884,6 +885,45 @@
   </si>
   <si>
     <t>Total Time</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_11032233-11151120_cluster-nondistinct/, ClustClosed_conf0.05_Buff1000,  ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=0.33 ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.05]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_11032233-11151120_cluster-nondistinct/, ClustClosed_conf0.1_Buff1000,  ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=0.33 ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.1]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_11032233-11151120_cluster-nondistinct/, ClustClosed_conf0.25_Buff1000,  ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=0.33 ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.25]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_11032233-11151120_cluster-nondistinct/, ClustClosed_conf0.2_Buff1000,  ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=0.33 ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.2]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_11032233-11151120_cluster-nondistinct/, ClustClosed_conf0.3_Buff1000,  ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=0.33 ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.3]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_11032233-11151120_cluster-nondistinct/, ClustClosed_conf0.4_Buff1000,  ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=0.33 ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.4]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_11032233-11151120_cluster-nondistinct/, ClustClosed_conf0.5_Buff1000,  ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=0.33 ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.5]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_11032233-11151120_cluster-nondistinct/, ClustClosed_conf0.6_Buff1000,  ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=0.33 ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.6]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_11032233-11151120_cluster-nondistinct/, ClustClosed_conf0.75_Buff1000,  ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=0.33 ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.75]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_11032233-11151120_cluster-nondistinct/, ClustClosed_conf0.7_Buff1000,  ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=0.33 ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.7]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_11032233-11151120_cluster-nondistinct/, ClustClosed_conf0.8_Buff1000,  ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=0.33 ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.8]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_11032233-11151120_cluster-nondistinct/, ClustClosed_conf0.95_Buff1000,  ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=0.33 ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.95]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_11032233-11151120_cluster-nondistinct/, ClustClosed_conf0.9_Buff1000,  ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=0.33 ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.9]</t>
   </si>
 </sst>
 </file>
@@ -1363,11 +1403,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2107985960"/>
-        <c:axId val="-2108314376"/>
+        <c:axId val="2120096040"/>
+        <c:axId val="2120106760"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2107985960"/>
+        <c:axId val="2120096040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1376,7 +1416,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2108314376"/>
+        <c:crossAx val="2120106760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1384,7 +1424,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2108314376"/>
+        <c:axId val="2120106760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1395,7 +1435,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2107985960"/>
+        <c:crossAx val="2120096040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1490,11 +1530,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2094175096"/>
-        <c:axId val="-2113792584"/>
+        <c:axId val="2122045080"/>
+        <c:axId val="2122048024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2094175096"/>
+        <c:axId val="2122045080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1503,7 +1543,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113792584"/>
+        <c:crossAx val="2122048024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1511,7 +1551,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2113792584"/>
+        <c:axId val="2122048024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1522,14 +1562,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2094175096"/>
+        <c:crossAx val="2122045080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1618,11 +1657,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2112627272"/>
-        <c:axId val="-2091814552"/>
+        <c:axId val="2122072872"/>
+        <c:axId val="2122075816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2112627272"/>
+        <c:axId val="2122072872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1631,7 +1670,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2091814552"/>
+        <c:crossAx val="2122075816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1639,7 +1678,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2091814552"/>
+        <c:axId val="2122075816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1650,14 +1689,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112627272"/>
+        <c:crossAx val="2122072872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1743,11 +1781,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2120641768"/>
-        <c:axId val="-2123228712"/>
+        <c:axId val="2122111704"/>
+        <c:axId val="2122114648"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2120641768"/>
+        <c:axId val="2122111704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1756,7 +1794,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123228712"/>
+        <c:crossAx val="2122114648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1764,7 +1802,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2123228712"/>
+        <c:axId val="2122114648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1775,14 +1813,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2120641768"/>
+        <c:crossAx val="2122111704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1868,11 +1905,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2123156040"/>
-        <c:axId val="-2122657560"/>
+        <c:axId val="2122138456"/>
+        <c:axId val="2122141400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2123156040"/>
+        <c:axId val="2122138456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1881,7 +1918,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122657560"/>
+        <c:crossAx val="2122141400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1889,7 +1926,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2122657560"/>
+        <c:axId val="2122141400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1900,14 +1937,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123156040"/>
+        <c:crossAx val="2122138456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2040,11 +2076,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2126733880"/>
-        <c:axId val="-2126879176"/>
+        <c:axId val="2122181032"/>
+        <c:axId val="2122184008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2126733880"/>
+        <c:axId val="2122181032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2053,7 +2089,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2126879176"/>
+        <c:crossAx val="2122184008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2061,7 +2097,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2126879176"/>
+        <c:axId val="2122184008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2072,14 +2108,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2126733880"/>
+        <c:crossAx val="2122181032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2162,8 +2197,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="75"/>
-        <c:axId val="-2120689560"/>
-        <c:axId val="-2122713976"/>
+        <c:axId val="2119191272"/>
+        <c:axId val="2119188280"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2328,11 +2363,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2120689560"/>
-        <c:axId val="-2122713976"/>
+        <c:axId val="2119191272"/>
+        <c:axId val="2119188280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2120689560"/>
+        <c:axId val="2119191272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2342,7 +2377,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122713976"/>
+        <c:crossAx val="2119188280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2350,7 +2385,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2122713976"/>
+        <c:axId val="2119188280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2361,14 +2396,13 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2120689560"/>
+        <c:crossAx val="2119191272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2582,11 +2616,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2127150040"/>
-        <c:axId val="-2126551624"/>
+        <c:axId val="2122460968"/>
+        <c:axId val="2122463944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2127150040"/>
+        <c:axId val="2122460968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2595,7 +2629,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2126551624"/>
+        <c:crossAx val="2122463944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2603,7 +2637,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2126551624"/>
+        <c:axId val="2122463944"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2638,7 +2672,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2127150040"/>
+        <c:crossAx val="2122460968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2855,11 +2889,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2123139944"/>
-        <c:axId val="-2057269512"/>
+        <c:axId val="2122499784"/>
+        <c:axId val="2122502760"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2123139944"/>
+        <c:axId val="2122499784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2868,7 +2902,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2057269512"/>
+        <c:crossAx val="2122502760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2876,7 +2910,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2057269512"/>
+        <c:axId val="2122502760"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2907,7 +2941,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123139944"/>
+        <c:crossAx val="2122499784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3155,11 +3189,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2113268984"/>
-        <c:axId val="-2113044520"/>
+        <c:axId val="2120151000"/>
+        <c:axId val="2120153976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2113268984"/>
+        <c:axId val="2120151000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3169,7 +3203,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113044520"/>
+        <c:crossAx val="2120153976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3177,7 +3211,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2113044520"/>
+        <c:axId val="2120153976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3188,7 +3222,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113268984"/>
+        <c:crossAx val="2120151000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3333,11 +3367,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2121514328"/>
-        <c:axId val="-2121410648"/>
+        <c:axId val="2120187352"/>
+        <c:axId val="2120190328"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2121514328"/>
+        <c:axId val="2120187352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3346,7 +3380,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121410648"/>
+        <c:crossAx val="2120190328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3354,7 +3388,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2121410648"/>
+        <c:axId val="2120190328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3365,14 +3399,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121514328"/>
+        <c:crossAx val="2120187352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3461,11 +3494,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2115574936"/>
-        <c:axId val="-2107860232"/>
+        <c:axId val="2119282744"/>
+        <c:axId val="2119280056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2115574936"/>
+        <c:axId val="2119282744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3474,7 +3507,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2107860232"/>
+        <c:crossAx val="2119280056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3482,7 +3515,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2107860232"/>
+        <c:axId val="2119280056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3493,14 +3526,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2115574936"/>
+        <c:crossAx val="2119282744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3684,11 +3716,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="100"/>
-        <c:axId val="-2086047096"/>
-        <c:axId val="-2084568328"/>
+        <c:axId val="2083483288"/>
+        <c:axId val="2083486408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2086047096"/>
+        <c:axId val="2083483288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3697,7 +3729,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2084568328"/>
+        <c:crossAx val="2083486408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3705,7 +3737,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2084568328"/>
+        <c:axId val="2083486408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3715,14 +3747,13 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2086047096"/>
+        <c:crossAx val="2083483288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3799,11 +3830,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2088297448"/>
-        <c:axId val="-2086302248"/>
+        <c:axId val="2082589768"/>
+        <c:axId val="2082579832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2088297448"/>
+        <c:axId val="2082589768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3812,7 +3843,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2086302248"/>
+        <c:crossAx val="2082579832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3820,7 +3851,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2086302248"/>
+        <c:axId val="2082579832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3831,14 +3862,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2088297448"/>
+        <c:crossAx val="2082589768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3977,11 +4007,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="100"/>
-        <c:axId val="-2081935608"/>
-        <c:axId val="-2114659656"/>
+        <c:axId val="2082546824"/>
+        <c:axId val="2082543688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2081935608"/>
+        <c:axId val="2082546824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3990,7 +4020,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2114659656"/>
+        <c:crossAx val="2082543688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3998,7 +4028,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114659656"/>
+        <c:axId val="2082543688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4008,14 +4038,13 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2081935608"/>
+        <c:crossAx val="2082546824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4045,7 +4074,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4203,11 +4231,11 @@
         </c:dLbls>
         <c:gapWidth val="95"/>
         <c:overlap val="100"/>
-        <c:axId val="-2116215704"/>
-        <c:axId val="-2116213832"/>
+        <c:axId val="2082491752"/>
+        <c:axId val="2082488616"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2116215704"/>
+        <c:axId val="2082491752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4216,7 +4244,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2116213832"/>
+        <c:crossAx val="2082488616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4224,7 +4252,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2116213832"/>
+        <c:axId val="2082488616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4234,7 +4262,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2116215704"/>
+        <c:crossAx val="2082491752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4245,7 +4273,6 @@
         <c:idx val="1"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4275,7 +4302,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4352,11 +4378,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2091895464"/>
-        <c:axId val="-2091204632"/>
+        <c:axId val="2119248920"/>
+        <c:axId val="2119245912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2091895464"/>
+        <c:axId val="2119248920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4365,7 +4391,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2091204632"/>
+        <c:crossAx val="2119245912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4373,7 +4399,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2091204632"/>
+        <c:axId val="2119245912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4384,14 +4410,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2091895464"/>
+        <c:crossAx val="2119248920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8414,7 +8439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:U20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+    <sheetView topLeftCell="B2" workbookViewId="0">
       <selection activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
@@ -8844,6 +8869,213 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:E16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="3" spans="2:5">
+      <c r="B3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" t="s">
+        <v>276</v>
+      </c>
+      <c r="C4">
+        <v>555</v>
+      </c>
+      <c r="D4">
+        <v>288.42882882882901</v>
+      </c>
+      <c r="E4">
+        <v>87.934090212784199</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" t="s">
+        <v>277</v>
+      </c>
+      <c r="C5">
+        <v>555</v>
+      </c>
+      <c r="D5">
+        <v>259.46126126126097</v>
+      </c>
+      <c r="E5">
+        <v>76.873752722318201</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C6">
+        <v>555</v>
+      </c>
+      <c r="D6">
+        <v>220.93153153153199</v>
+      </c>
+      <c r="E6">
+        <v>63.676378855777202</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" t="s">
+        <v>279</v>
+      </c>
+      <c r="C7">
+        <v>555</v>
+      </c>
+      <c r="D7">
+        <v>227.99459459459499</v>
+      </c>
+      <c r="E7">
+        <v>68.089066004440198</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" t="s">
+        <v>280</v>
+      </c>
+      <c r="C8">
+        <v>555</v>
+      </c>
+      <c r="D8">
+        <v>217.54234234234201</v>
+      </c>
+      <c r="E8">
+        <v>61.451776681552602</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="B9" t="s">
+        <v>281</v>
+      </c>
+      <c r="C9">
+        <v>555</v>
+      </c>
+      <c r="D9">
+        <v>212.70810810810801</v>
+      </c>
+      <c r="E9">
+        <v>56.896490877839902</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="B10" t="s">
+        <v>282</v>
+      </c>
+      <c r="C10">
+        <v>555</v>
+      </c>
+      <c r="D10">
+        <v>210.52972972973001</v>
+      </c>
+      <c r="E10">
+        <v>53.805845968594703</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="B11" t="s">
+        <v>283</v>
+      </c>
+      <c r="C11">
+        <v>555</v>
+      </c>
+      <c r="D11">
+        <v>216.97117117117099</v>
+      </c>
+      <c r="E11">
+        <v>60.9256447273969</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="B12" t="s">
+        <v>284</v>
+      </c>
+      <c r="C12">
+        <v>555</v>
+      </c>
+      <c r="D12">
+        <v>228.79819819819801</v>
+      </c>
+      <c r="E12">
+        <v>67.802343311131196</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="B13" t="s">
+        <v>285</v>
+      </c>
+      <c r="C13">
+        <v>555</v>
+      </c>
+      <c r="D13">
+        <v>224.24684684684701</v>
+      </c>
+      <c r="E13">
+        <v>65.586622276407297</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5">
+      <c r="B14" t="s">
+        <v>286</v>
+      </c>
+      <c r="C14">
+        <v>555</v>
+      </c>
+      <c r="D14">
+        <v>235.53513513513499</v>
+      </c>
+      <c r="E14">
+        <v>71.048949222888993</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5">
+      <c r="B15" t="s">
+        <v>287</v>
+      </c>
+      <c r="C15">
+        <v>555</v>
+      </c>
+      <c r="D15">
+        <v>297.241441441441</v>
+      </c>
+      <c r="E15">
+        <v>90.125580725827206</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5">
+      <c r="B16" t="s">
+        <v>288</v>
+      </c>
+      <c r="C16">
+        <v>555</v>
+      </c>
+      <c r="D16">
+        <v>268.50990990990999</v>
+      </c>
+      <c r="E16">
+        <v>80.000098098941393</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>